<commit_message>
Ich habe an meinem Gantchart gearbeitet
</commit_message>
<xml_diff>
--- a/docs/EchoPlay_Gantchart_250514.xlsx
+++ b/docs/EchoPlay_Gantchart_250514.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED1B8E1-01DD-4E2C-BCBC-156AC4178406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37870930-5538-47B6-A78B-9AA0DE282262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-130" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplan" sheetId="11" r:id="rId1"/>
@@ -1303,35 +1303,35 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="9" fillId="3" borderId="2" xfId="12" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="3" borderId="2" xfId="12" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="3" borderId="2" xfId="12" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="3" borderId="2" xfId="12" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="3" borderId="2" xfId="12" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="3" borderId="2" xfId="12" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1942,26 +1942,26 @@
   </sheetPr>
   <dimension ref="A1:BL27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="67" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="44" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.5703125" customWidth="1"/>
-    <col min="69" max="70" width="10.28515625"/>
+    <col min="1" max="1" width="2.7265625" style="44" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="2.7265625" customWidth="1"/>
+    <col min="8" max="8" width="6.1796875" hidden="1" customWidth="1"/>
+    <col min="9" max="64" width="2.54296875" customWidth="1"/>
+    <col min="69" max="70" width="10.26953125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
@@ -1975,7 +1975,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="64"/>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
@@ -1988,7 +1988,7 @@
       <c r="D2" s="84"/>
       <c r="I2" s="65"/>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="44" t="s">
         <v>2</v>
       </c>
@@ -1999,104 +1999,104 @@
         <v>44</v>
       </c>
       <c r="D3" s="86"/>
-      <c r="E3" s="92">
+      <c r="E3" s="91">
         <v>45733</v>
       </c>
-      <c r="F3" s="92"/>
+      <c r="F3" s="91"/>
     </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="88"/>
+      <c r="D4" s="96"/>
       <c r="E4" s="7">
-        <v>4</v>
-      </c>
-      <c r="I4" s="89">
+        <v>6</v>
+      </c>
+      <c r="I4" s="92">
         <f>I5</f>
-        <v>45754</v>
-      </c>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="89">
+        <v>45768</v>
+      </c>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="94"/>
+      <c r="P4" s="92">
         <f>P5</f>
-        <v>45761</v>
-      </c>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="91"/>
-      <c r="W4" s="89">
+        <v>45775</v>
+      </c>
+      <c r="Q4" s="93"/>
+      <c r="R4" s="93"/>
+      <c r="S4" s="93"/>
+      <c r="T4" s="93"/>
+      <c r="U4" s="93"/>
+      <c r="V4" s="94"/>
+      <c r="W4" s="92">
         <f>W5</f>
-        <v>45768</v>
-      </c>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-      <c r="AB4" s="90"/>
-      <c r="AC4" s="91"/>
-      <c r="AD4" s="89">
+        <v>45782</v>
+      </c>
+      <c r="X4" s="93"/>
+      <c r="Y4" s="93"/>
+      <c r="Z4" s="93"/>
+      <c r="AA4" s="93"/>
+      <c r="AB4" s="93"/>
+      <c r="AC4" s="94"/>
+      <c r="AD4" s="92">
         <f>AD5</f>
-        <v>45775</v>
-      </c>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="90"/>
-      <c r="AG4" s="90"/>
-      <c r="AH4" s="90"/>
-      <c r="AI4" s="90"/>
-      <c r="AJ4" s="91"/>
-      <c r="AK4" s="89">
+        <v>45789</v>
+      </c>
+      <c r="AE4" s="93"/>
+      <c r="AF4" s="93"/>
+      <c r="AG4" s="93"/>
+      <c r="AH4" s="93"/>
+      <c r="AI4" s="93"/>
+      <c r="AJ4" s="94"/>
+      <c r="AK4" s="92">
         <f>AK5</f>
-        <v>45782</v>
-      </c>
-      <c r="AL4" s="90"/>
-      <c r="AM4" s="90"/>
-      <c r="AN4" s="90"/>
-      <c r="AO4" s="90"/>
-      <c r="AP4" s="90"/>
-      <c r="AQ4" s="91"/>
-      <c r="AR4" s="89">
+        <v>45796</v>
+      </c>
+      <c r="AL4" s="93"/>
+      <c r="AM4" s="93"/>
+      <c r="AN4" s="93"/>
+      <c r="AO4" s="93"/>
+      <c r="AP4" s="93"/>
+      <c r="AQ4" s="94"/>
+      <c r="AR4" s="92">
         <f>AR5</f>
-        <v>45789</v>
-      </c>
-      <c r="AS4" s="90"/>
-      <c r="AT4" s="90"/>
-      <c r="AU4" s="90"/>
-      <c r="AV4" s="90"/>
-      <c r="AW4" s="90"/>
-      <c r="AX4" s="91"/>
-      <c r="AY4" s="89">
+        <v>45803</v>
+      </c>
+      <c r="AS4" s="93"/>
+      <c r="AT4" s="93"/>
+      <c r="AU4" s="93"/>
+      <c r="AV4" s="93"/>
+      <c r="AW4" s="93"/>
+      <c r="AX4" s="94"/>
+      <c r="AY4" s="92">
         <f>AY5</f>
-        <v>45796</v>
-      </c>
-      <c r="AZ4" s="90"/>
-      <c r="BA4" s="90"/>
-      <c r="BB4" s="90"/>
-      <c r="BC4" s="90"/>
-      <c r="BD4" s="90"/>
-      <c r="BE4" s="91"/>
-      <c r="BF4" s="89">
+        <v>45810</v>
+      </c>
+      <c r="AZ4" s="93"/>
+      <c r="BA4" s="93"/>
+      <c r="BB4" s="93"/>
+      <c r="BC4" s="93"/>
+      <c r="BD4" s="93"/>
+      <c r="BE4" s="94"/>
+      <c r="BF4" s="92">
         <f>BF5</f>
-        <v>45803</v>
-      </c>
-      <c r="BG4" s="90"/>
-      <c r="BH4" s="90"/>
-      <c r="BI4" s="90"/>
-      <c r="BJ4" s="90"/>
-      <c r="BK4" s="90"/>
-      <c r="BL4" s="91"/>
+        <v>45817</v>
+      </c>
+      <c r="BG4" s="93"/>
+      <c r="BH4" s="93"/>
+      <c r="BI4" s="93"/>
+      <c r="BJ4" s="93"/>
+      <c r="BK4" s="93"/>
+      <c r="BL4" s="94"/>
     </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="45" t="s">
         <v>4</v>
       </c>
@@ -2108,230 +2108,230 @@
       <c r="G5" s="63"/>
       <c r="I5" s="81">
         <f>Projektanfang-WEEKDAY(Projektanfang,1)+2+7*(Anzeigewoche-1)</f>
-        <v>45754</v>
+        <v>45768</v>
       </c>
       <c r="J5" s="82">
         <f>I5+1</f>
-        <v>45755</v>
+        <v>45769</v>
       </c>
       <c r="K5" s="82">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
-        <v>45756</v>
+        <v>45770</v>
       </c>
       <c r="L5" s="82">
         <f t="shared" si="0"/>
-        <v>45757</v>
+        <v>45771</v>
       </c>
       <c r="M5" s="82">
         <f t="shared" si="0"/>
-        <v>45758</v>
+        <v>45772</v>
       </c>
       <c r="N5" s="82">
         <f t="shared" si="0"/>
-        <v>45759</v>
+        <v>45773</v>
       </c>
       <c r="O5" s="83">
         <f t="shared" si="0"/>
-        <v>45760</v>
+        <v>45774</v>
       </c>
       <c r="P5" s="81">
         <f>O5+1</f>
-        <v>45761</v>
+        <v>45775</v>
       </c>
       <c r="Q5" s="82">
         <f>P5+1</f>
-        <v>45762</v>
+        <v>45776</v>
       </c>
       <c r="R5" s="82">
         <f t="shared" si="0"/>
-        <v>45763</v>
+        <v>45777</v>
       </c>
       <c r="S5" s="82">
         <f t="shared" si="0"/>
-        <v>45764</v>
+        <v>45778</v>
       </c>
       <c r="T5" s="82">
         <f t="shared" si="0"/>
-        <v>45765</v>
+        <v>45779</v>
       </c>
       <c r="U5" s="82">
         <f t="shared" si="0"/>
-        <v>45766</v>
+        <v>45780</v>
       </c>
       <c r="V5" s="83">
         <f t="shared" si="0"/>
-        <v>45767</v>
+        <v>45781</v>
       </c>
       <c r="W5" s="81">
         <f>V5+1</f>
-        <v>45768</v>
+        <v>45782</v>
       </c>
       <c r="X5" s="82">
         <f>W5+1</f>
-        <v>45769</v>
+        <v>45783</v>
       </c>
       <c r="Y5" s="82">
         <f t="shared" si="0"/>
-        <v>45770</v>
+        <v>45784</v>
       </c>
       <c r="Z5" s="82">
         <f t="shared" si="0"/>
-        <v>45771</v>
+        <v>45785</v>
       </c>
       <c r="AA5" s="82">
         <f t="shared" si="0"/>
-        <v>45772</v>
+        <v>45786</v>
       </c>
       <c r="AB5" s="82">
         <f t="shared" si="0"/>
-        <v>45773</v>
+        <v>45787</v>
       </c>
       <c r="AC5" s="83">
         <f t="shared" si="0"/>
-        <v>45774</v>
+        <v>45788</v>
       </c>
       <c r="AD5" s="81">
         <f>AC5+1</f>
-        <v>45775</v>
+        <v>45789</v>
       </c>
       <c r="AE5" s="82">
         <f>AD5+1</f>
-        <v>45776</v>
+        <v>45790</v>
       </c>
       <c r="AF5" s="82">
         <f t="shared" si="0"/>
-        <v>45777</v>
+        <v>45791</v>
       </c>
       <c r="AG5" s="82">
         <f t="shared" si="0"/>
-        <v>45778</v>
+        <v>45792</v>
       </c>
       <c r="AH5" s="82">
         <f t="shared" si="0"/>
-        <v>45779</v>
+        <v>45793</v>
       </c>
       <c r="AI5" s="82">
         <f t="shared" si="0"/>
-        <v>45780</v>
+        <v>45794</v>
       </c>
       <c r="AJ5" s="83">
         <f t="shared" si="0"/>
-        <v>45781</v>
+        <v>45795</v>
       </c>
       <c r="AK5" s="81">
         <f>AJ5+1</f>
-        <v>45782</v>
+        <v>45796</v>
       </c>
       <c r="AL5" s="82">
         <f>AK5+1</f>
-        <v>45783</v>
+        <v>45797</v>
       </c>
       <c r="AM5" s="82">
         <f t="shared" si="0"/>
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="AN5" s="82">
         <f t="shared" si="0"/>
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="AO5" s="82">
         <f t="shared" si="0"/>
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="AP5" s="82">
         <f t="shared" si="0"/>
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="AQ5" s="83">
         <f t="shared" si="0"/>
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="AR5" s="81">
         <f>AQ5+1</f>
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="AS5" s="82">
         <f>AR5+1</f>
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="AT5" s="82">
         <f t="shared" si="0"/>
-        <v>45791</v>
+        <v>45805</v>
       </c>
       <c r="AU5" s="82">
         <f t="shared" si="0"/>
-        <v>45792</v>
+        <v>45806</v>
       </c>
       <c r="AV5" s="82">
         <f t="shared" si="0"/>
-        <v>45793</v>
+        <v>45807</v>
       </c>
       <c r="AW5" s="82">
         <f t="shared" si="0"/>
-        <v>45794</v>
+        <v>45808</v>
       </c>
       <c r="AX5" s="83">
         <f t="shared" si="0"/>
-        <v>45795</v>
+        <v>45809</v>
       </c>
       <c r="AY5" s="81">
         <f>AX5+1</f>
-        <v>45796</v>
+        <v>45810</v>
       </c>
       <c r="AZ5" s="82">
         <f>AY5+1</f>
-        <v>45797</v>
+        <v>45811</v>
       </c>
       <c r="BA5" s="82">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>45798</v>
+        <v>45812</v>
       </c>
       <c r="BB5" s="82">
         <f t="shared" si="1"/>
-        <v>45799</v>
+        <v>45813</v>
       </c>
       <c r="BC5" s="82">
         <f t="shared" si="1"/>
-        <v>45800</v>
+        <v>45814</v>
       </c>
       <c r="BD5" s="82">
         <f t="shared" si="1"/>
-        <v>45801</v>
+        <v>45815</v>
       </c>
       <c r="BE5" s="83">
         <f t="shared" si="1"/>
-        <v>45802</v>
+        <v>45816</v>
       </c>
       <c r="BF5" s="81">
         <f>BE5+1</f>
-        <v>45803</v>
+        <v>45817</v>
       </c>
       <c r="BG5" s="82">
         <f>BF5+1</f>
-        <v>45804</v>
+        <v>45818</v>
       </c>
       <c r="BH5" s="82">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
-        <v>45805</v>
+        <v>45819</v>
       </c>
       <c r="BI5" s="82">
         <f t="shared" si="2"/>
-        <v>45806</v>
+        <v>45820</v>
       </c>
       <c r="BJ5" s="82">
         <f t="shared" si="2"/>
-        <v>45807</v>
+        <v>45821</v>
       </c>
       <c r="BK5" s="82">
         <f t="shared" si="2"/>
-        <v>45808</v>
+        <v>45822</v>
       </c>
       <c r="BL5" s="83">
         <f t="shared" si="2"/>
-        <v>45809</v>
+        <v>45823</v>
       </c>
     </row>
-    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="44" t="s">
         <v>6</v>
       </c>
@@ -2646,7 +2646,7 @@
       <c r="BK7" s="30"/>
       <c r="BL7" s="30"/>
     </row>
-    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="45" t="s">
         <v>7</v>
       </c>
@@ -2719,7 +2719,7 @@
       <c r="BK8" s="30"/>
       <c r="BL8" s="30"/>
     </row>
-    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="45" t="s">
         <v>8</v>
       </c>
@@ -2801,7 +2801,7 @@
       <c r="BK9" s="30"/>
       <c r="BL9" s="30"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="45" t="s">
         <v>9</v>
       </c>
@@ -2882,7 +2882,7 @@
       <c r="BK10" s="30"/>
       <c r="BL10" s="30"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="44"/>
       <c r="B11" s="59" t="s">
         <v>48</v>
@@ -2961,7 +2961,7 @@
       <c r="BK11" s="30"/>
       <c r="BL11" s="30"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="45" t="s">
         <v>10</v>
       </c>
@@ -3034,7 +3034,7 @@
       <c r="BK12" s="30"/>
       <c r="BL12" s="30"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="45"/>
       <c r="B13" s="60" t="s">
         <v>49</v>
@@ -3043,7 +3043,7 @@
         <v>44</v>
       </c>
       <c r="D13" s="19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E13" s="72">
         <v>45748</v>
@@ -3113,7 +3113,7 @@
       <c r="BK13" s="30"/>
       <c r="BL13" s="30"/>
     </row>
-    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="44"/>
       <c r="B14" s="60" t="s">
         <v>50</v>
@@ -3192,7 +3192,7 @@
       <c r="BK14" s="30"/>
       <c r="BL14" s="30"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="44" t="s">
         <v>11</v>
       </c>
@@ -3265,7 +3265,7 @@
       <c r="BK15" s="30"/>
       <c r="BL15" s="30"/>
     </row>
-    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="44"/>
       <c r="B16" s="61" t="s">
         <v>51</v>
@@ -3344,7 +3344,7 @@
       <c r="BK16" s="30"/>
       <c r="BL16" s="30"/>
     </row>
-    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="44" t="s">
         <v>11</v>
       </c>
@@ -3417,7 +3417,7 @@
       <c r="BK17" s="30"/>
       <c r="BL17" s="30"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="44"/>
       <c r="B18" s="62" t="s">
         <v>52</v>
@@ -3496,7 +3496,7 @@
       <c r="BK18" s="30"/>
       <c r="BL18" s="30"/>
     </row>
-    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="44"/>
       <c r="B19" s="62" t="s">
         <v>53</v>
@@ -3575,7 +3575,7 @@
       <c r="BK19" s="30"/>
       <c r="BL19" s="30"/>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="44"/>
       <c r="B20" s="14" t="s">
         <v>54</v>
@@ -3643,21 +3643,21 @@
       <c r="BK20" s="30"/>
       <c r="BL20" s="30"/>
     </row>
-    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="44"/>
       <c r="B21" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="96" t="s">
+      <c r="C21" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="93">
+      <c r="D21" s="87">
         <v>0</v>
       </c>
-      <c r="E21" s="95">
+      <c r="E21" s="89">
         <v>45813</v>
       </c>
-      <c r="F21" s="95">
+      <c r="F21" s="89">
         <v>45820</v>
       </c>
       <c r="G21" s="13"/>
@@ -3719,7 +3719,7 @@
       <c r="BK21" s="30"/>
       <c r="BL21" s="30"/>
     </row>
-    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="44"/>
       <c r="B22" s="14" t="s">
         <v>43</v>
@@ -3787,21 +3787,21 @@
       <c r="BK22" s="30"/>
       <c r="BL22" s="30"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="44"/>
       <c r="B23" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="96" t="s">
+      <c r="C23" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="93">
+      <c r="D23" s="87">
         <v>0</v>
       </c>
-      <c r="E23" s="94">
+      <c r="E23" s="88">
         <v>45824</v>
       </c>
-      <c r="F23" s="95">
+      <c r="F23" s="89">
         <v>45824</v>
       </c>
       <c r="G23" s="13"/>
@@ -3863,7 +3863,7 @@
       <c r="BK23" s="30"/>
       <c r="BL23" s="30"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="45" t="s">
         <v>12</v>
       </c>
@@ -3936,28 +3936,28 @@
       <c r="BK24" s="32"/>
       <c r="BL24" s="32"/>
     </row>
-    <row r="25" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C26" s="11"/>
       <c r="F26" s="46"/>
     </row>
-    <row r="27" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C27" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D19 D24">
     <cfRule type="dataBar" priority="14">
@@ -4027,86 +4027,86 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="87.140625" style="34" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="87.1796875" style="34" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:2" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" s="36" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="35"/>
     </row>
-    <row r="3" spans="1:2" s="40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="40" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="66" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="41"/>
     </row>
-    <row r="4" spans="1:2" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A4" s="38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="34" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="34" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="43" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A8" s="38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A9" s="39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="34" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="34" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="42" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A11" s="38" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.3">
       <c r="A12" s="39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="34" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" s="34" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A14" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A16" s="39" t="s">
         <v>38</v>
       </c>
@@ -4125,12 +4125,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4422,29 +4433,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4471,13 +4475,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>